<commit_message>
przelewy wychodzące do SŁonka
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki.xlsx
+++ b/plan/Mati - wydatki.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Data</t>
   </si>
@@ -53,12 +52,66 @@
   </si>
   <si>
     <t>Glapa</t>
+  </si>
+  <si>
+    <t>Przelewy z mbanku</t>
+  </si>
+  <si>
+    <t>26-07-2012</t>
+  </si>
+  <si>
+    <t>TYSIAK</t>
+  </si>
+  <si>
+    <t>27-08-2012</t>
+  </si>
+  <si>
+    <t>19-09-2012</t>
+  </si>
+  <si>
+    <t>tysiąć</t>
+  </si>
+  <si>
+    <t>04-10-2012</t>
+  </si>
+  <si>
+    <t>damy radę</t>
+  </si>
+  <si>
+    <t>23-11-2012</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>tytuł</t>
+  </si>
+  <si>
+    <t>kwota</t>
+  </si>
+  <si>
+    <t>Przelewy z polbanku</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Przelewy z eb</t>
+  </si>
+  <si>
+    <t>15-10-2012</t>
+  </si>
+  <si>
+    <t>tysiąc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;zł&quot;;[Red]\-#,##0\ &quot;zł&quot;"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -86,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -94,15 +147,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -397,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -525,99 +607,201 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="C13" s="2"/>
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="C14" s="2"/>
+      <c r="A14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1000</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="C15" s="2"/>
+      <c r="A15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="9">
+        <v>2500</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2500</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="C16" s="2"/>
+      <c r="A16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1000</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="3:5">
-      <c r="C17" s="2"/>
+    <row r="17" spans="1:5">
+      <c r="A17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1000</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="3:5">
-      <c r="C18" s="2"/>
+    <row r="18" spans="1:5">
+      <c r="A18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="10">
+        <v>500</v>
+      </c>
+      <c r="C18" s="8">
+        <v>500</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="3:5">
+    <row r="19" spans="1:5">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="3:5">
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="3:5">
-      <c r="C21" s="2"/>
+    <row r="21" spans="1:5">
+      <c r="A21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="3:5">
-      <c r="C22" s="2"/>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="3:5">
-      <c r="C23" s="2"/>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="3:5">
+    <row r="24" spans="1:5">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="3:5">
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="3:5">
-      <c r="C26" s="2"/>
+    <row r="26" spans="1:5">
+      <c r="A26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="3:5">
-      <c r="C27" s="2"/>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1000</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="3:5">
+    <row r="28" spans="1:5">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="3:5">
+    <row r="29" spans="1:5">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="3:5">
+    <row r="30" spans="1:5">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update wydatki - juz w trakcie budowy
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki.xlsx
+++ b/plan/Mati - wydatki.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Data</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Partyka - update projektu kanalizacji</t>
+  </si>
+  <si>
+    <t>2013-07-xx</t>
+  </si>
+  <si>
+    <t>Geodeta cz.1</t>
+  </si>
+  <si>
+    <t>Geodeta cz.2</t>
+  </si>
+  <si>
+    <t>Piasek</t>
   </si>
 </sst>
 </file>
@@ -460,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -581,7 +593,7 @@
         <v>1500</v>
       </c>
       <c r="E7" s="11">
-        <f t="shared" ref="E7:E19" si="0">C7+D7</f>
+        <f t="shared" ref="E7:E22" si="0">C7+D7</f>
         <v>3000</v>
       </c>
     </row>
@@ -802,25 +814,58 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="5"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="A20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="14">
+        <v>0</v>
+      </c>
+      <c r="D20" s="14">
+        <v>400</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="5"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="A21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="14">
+        <v>0</v>
+      </c>
+      <c r="D21" s="14">
+        <v>650</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>650</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="5"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="A22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="14">
+        <v>2000</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5800</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>7800</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="5"/>

</xml_diff>

<commit_message>
nowe faktury z Manexu
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki.xlsx
+++ b/plan/Mati - wydatki.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Data</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>Stal</t>
+  </si>
+  <si>
+    <t>4877/T/08/2013</t>
+  </si>
+  <si>
+    <t>Rura woda</t>
+  </si>
+  <si>
+    <t>4916/T/08/2013</t>
+  </si>
+  <si>
+    <t>4969/T/08/2013</t>
+  </si>
+  <si>
+    <t>Styropian</t>
   </si>
 </sst>
 </file>
@@ -1048,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G4"/>
+  <dimension ref="A2:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1129,6 +1144,57 @@
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="12">
+        <v>41498</v>
+      </c>
+      <c r="B5" s="12">
+        <v>41501</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="13">
+        <v>19.079999999999998</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="12">
+        <v>41498</v>
+      </c>
+      <c r="B6" s="12">
+        <v>41501</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="13">
+        <v>115.01</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="12">
+        <v>41499</v>
+      </c>
+      <c r="B7" s="12">
+        <v>41502</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="13">
+        <v>8280.36</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
szablony do faktur Tauron/Zgk
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki.xlsx
+++ b/plan/Mati - wydatki.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="13020" windowHeight="2895" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="13020" windowHeight="2895" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Wydatki" sheetId="1" r:id="rId1"/>
     <sheet name="Faktury Manex" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="Rachunki Tauron" sheetId="3" r:id="rId3"/>
+    <sheet name="Rachunki ZGK" sheetId="4" r:id="rId4"/>
+    <sheet name="Podatek Kąty" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Data</t>
   </si>
@@ -154,6 +156,24 @@
   </si>
   <si>
     <t>SUMA</t>
+  </si>
+  <si>
+    <t>Nr faktury</t>
+  </si>
+  <si>
+    <t>Zapłacono</t>
+  </si>
+  <si>
+    <t>559021187/3/s</t>
+  </si>
+  <si>
+    <t>559021187/4/s</t>
+  </si>
+  <si>
+    <t>Kwota przelewu</t>
+  </si>
+  <si>
+    <t>Termin zapłaty</t>
   </si>
 </sst>
 </file>
@@ -230,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -246,6 +266,7 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -268,6 +289,49 @@
     <tableColumn id="7" name="Konto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B2:F14" totalsRowShown="0">
+  <autoFilter ref="B2:F14">
+    <filterColumn colId="4"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Data płatności"/>
+    <tableColumn id="2" name="Nr faktury"/>
+    <tableColumn id="3" name="Kwota"/>
+    <tableColumn id="4" name="Zapłacono"/>
+    <tableColumn id="12" name="Kwota przelewu"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="B2:G12" totalsRowShown="0">
+  <autoFilter ref="B2:G12"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Data płatności"/>
+    <tableColumn id="2" name="Kwota"/>
+    <tableColumn id="3" name="Opis"/>
+    <tableColumn id="4" name="Nr faktury"/>
+    <tableColumn id="5" name="Zapłacono"/>
+    <tableColumn id="6" name="Kwota przelewu"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela46" displayName="Tabela46" ref="B2:D9" totalsRowShown="0">
+  <autoFilter ref="B2:D9"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Termin zapłaty"/>
+    <tableColumn id="2" name="Kwota"/>
+    <tableColumn id="3" name="Zapłacono"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1069,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1225,13 +1289,177 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="15">
+        <v>41442</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3">
+        <v>58.23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="15">
+        <v>41470</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>58.23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="15">
+        <v>41348</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="15">
+        <v>41409</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="15">
+        <v>41532</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="15">
+        <v>41593</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
kolejna faktura za stal
</commit_message>
<xml_diff>
--- a/plan/Mati - wydatki.xlsx
+++ b/plan/Mati - wydatki.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>Data</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>5017/T/08/2013</t>
+  </si>
+  <si>
+    <t>5042/T/08/2013</t>
   </si>
 </sst>
 </file>
@@ -206,7 +209,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="8" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -214,6 +216,7 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -266,10 +269,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1139,7 +1142,7 @@
   <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1177,125 +1180,125 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="10">
+      <c r="A3" s="12">
         <v>41494</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="12">
         <v>41497</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="13">
         <v>1510.21</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="12">
         <v>41495</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="14">
+      <c r="A4" s="12">
         <v>41494</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="12">
         <v>41501</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="13">
         <v>5878.78</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="12">
         <v>41501</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="14">
+      <c r="A5" s="12">
         <v>41498</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="12">
         <v>41501</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="13">
         <v>19.079999999999998</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>41501</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="14">
+      <c r="A6" s="12">
         <v>41498</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>41501</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="13">
         <v>115.01</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="12">
         <v>41501</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="14">
+      <c r="A7" s="12">
         <v>41499</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="12">
         <v>41502</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <v>8280.36</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="12">
         <v>41501</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="13">
+      <c r="A8" s="11">
         <v>41502</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>41505</v>
       </c>
       <c r="C8" t="s">
@@ -1307,26 +1310,43 @@
       <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="11">
         <v>41502</v>
       </c>
       <c r="G8" t="s">
         <v>52</v>
       </c>
     </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="14">
+        <v>41502</v>
+      </c>
+      <c r="B9" s="14">
+        <v>41509</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="15">
+        <v>512.29999999999995</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="10">
         <f>SUM(D3:D15)</f>
-        <v>17460.87</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+        <v>17973.169999999998</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1372,7 +1392,7 @@
       </c>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="13">
+      <c r="B3" s="11">
         <v>41442</v>
       </c>
       <c r="C3" t="s">
@@ -1381,7 +1401,7 @@
       <c r="D3">
         <v>58.23</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <v>41501</v>
       </c>
       <c r="F3">
@@ -1389,7 +1409,7 @@
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="13">
+      <c r="B4" s="11">
         <v>41470</v>
       </c>
       <c r="C4" t="s">
@@ -1398,7 +1418,7 @@
       <c r="D4">
         <v>58.23</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="11">
         <v>41501</v>
       </c>
       <c r="F4">
@@ -1406,202 +1426,202 @@
       </c>
     </row>
     <row r="27" spans="4:4">
-      <c r="D27" s="13"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" spans="4:4">
-      <c r="D28" s="13"/>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" spans="4:4">
-      <c r="D29" s="13"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="4:4">
-      <c r="D30" s="13"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="4:4">
-      <c r="D31" s="13"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="4:4">
-      <c r="D32" s="13"/>
+      <c r="D32" s="11"/>
     </row>
     <row r="33" spans="4:4">
-      <c r="D33" s="13"/>
+      <c r="D33" s="11"/>
     </row>
     <row r="34" spans="4:4">
-      <c r="D34" s="13"/>
+      <c r="D34" s="11"/>
     </row>
     <row r="35" spans="4:4">
-      <c r="D35" s="13"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="4:4">
-      <c r="D36" s="13"/>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" spans="4:4">
-      <c r="D37" s="13"/>
+      <c r="D37" s="11"/>
     </row>
     <row r="38" spans="4:4">
-      <c r="D38" s="13"/>
+      <c r="D38" s="11"/>
     </row>
     <row r="39" spans="4:4">
-      <c r="D39" s="13"/>
+      <c r="D39" s="11"/>
     </row>
     <row r="40" spans="4:4">
-      <c r="D40" s="13"/>
+      <c r="D40" s="11"/>
     </row>
     <row r="41" spans="4:4">
-      <c r="D41" s="13"/>
+      <c r="D41" s="11"/>
     </row>
     <row r="42" spans="4:4">
-      <c r="D42" s="13"/>
+      <c r="D42" s="11"/>
     </row>
     <row r="43" spans="4:4">
-      <c r="D43" s="13"/>
+      <c r="D43" s="11"/>
     </row>
     <row r="44" spans="4:4">
-      <c r="D44" s="13"/>
+      <c r="D44" s="11"/>
     </row>
     <row r="45" spans="4:4">
-      <c r="D45" s="13"/>
+      <c r="D45" s="11"/>
     </row>
     <row r="46" spans="4:4">
-      <c r="D46" s="13"/>
+      <c r="D46" s="11"/>
     </row>
     <row r="47" spans="4:4">
-      <c r="D47" s="13"/>
+      <c r="D47" s="11"/>
     </row>
     <row r="48" spans="4:4">
-      <c r="D48" s="13"/>
+      <c r="D48" s="11"/>
     </row>
     <row r="49" spans="4:4">
-      <c r="D49" s="13"/>
+      <c r="D49" s="11"/>
     </row>
     <row r="50" spans="4:4">
-      <c r="D50" s="13"/>
+      <c r="D50" s="11"/>
     </row>
     <row r="51" spans="4:4">
-      <c r="D51" s="13"/>
+      <c r="D51" s="11"/>
     </row>
     <row r="52" spans="4:4">
-      <c r="D52" s="13"/>
+      <c r="D52" s="11"/>
     </row>
     <row r="53" spans="4:4">
-      <c r="D53" s="13"/>
+      <c r="D53" s="11"/>
     </row>
     <row r="54" spans="4:4">
-      <c r="D54" s="13"/>
+      <c r="D54" s="11"/>
     </row>
     <row r="55" spans="4:4">
-      <c r="D55" s="13"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="4:4">
-      <c r="D56" s="13"/>
+      <c r="D56" s="11"/>
     </row>
     <row r="57" spans="4:4">
-      <c r="D57" s="13"/>
+      <c r="D57" s="11"/>
     </row>
     <row r="58" spans="4:4">
-      <c r="D58" s="13"/>
+      <c r="D58" s="11"/>
     </row>
     <row r="59" spans="4:4">
-      <c r="D59" s="13"/>
+      <c r="D59" s="11"/>
     </row>
     <row r="60" spans="4:4">
-      <c r="D60" s="13"/>
+      <c r="D60" s="11"/>
     </row>
     <row r="61" spans="4:4">
-      <c r="D61" s="13"/>
+      <c r="D61" s="11"/>
     </row>
     <row r="62" spans="4:4">
-      <c r="D62" s="13"/>
+      <c r="D62" s="11"/>
     </row>
     <row r="63" spans="4:4">
-      <c r="D63" s="13"/>
+      <c r="D63" s="11"/>
     </row>
     <row r="64" spans="4:4">
-      <c r="D64" s="13"/>
+      <c r="D64" s="11"/>
     </row>
     <row r="65" spans="4:4">
-      <c r="D65" s="13"/>
+      <c r="D65" s="11"/>
     </row>
     <row r="66" spans="4:4">
-      <c r="D66" s="13"/>
+      <c r="D66" s="11"/>
     </row>
     <row r="67" spans="4:4">
-      <c r="D67" s="13"/>
+      <c r="D67" s="11"/>
     </row>
     <row r="68" spans="4:4">
-      <c r="D68" s="13"/>
+      <c r="D68" s="11"/>
     </row>
     <row r="69" spans="4:4">
-      <c r="D69" s="13"/>
+      <c r="D69" s="11"/>
     </row>
     <row r="70" spans="4:4">
-      <c r="D70" s="13"/>
+      <c r="D70" s="11"/>
     </row>
     <row r="71" spans="4:4">
-      <c r="D71" s="13"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="4:4">
-      <c r="D72" s="13"/>
+      <c r="D72" s="11"/>
     </row>
     <row r="73" spans="4:4">
-      <c r="D73" s="13"/>
+      <c r="D73" s="11"/>
     </row>
     <row r="74" spans="4:4">
-      <c r="D74" s="13"/>
+      <c r="D74" s="11"/>
     </row>
     <row r="75" spans="4:4">
-      <c r="D75" s="13"/>
+      <c r="D75" s="11"/>
     </row>
     <row r="76" spans="4:4">
-      <c r="D76" s="13"/>
+      <c r="D76" s="11"/>
     </row>
     <row r="77" spans="4:4">
-      <c r="D77" s="13"/>
+      <c r="D77" s="11"/>
     </row>
     <row r="78" spans="4:4">
-      <c r="D78" s="13"/>
+      <c r="D78" s="11"/>
     </row>
     <row r="79" spans="4:4">
-      <c r="D79" s="13"/>
+      <c r="D79" s="11"/>
     </row>
     <row r="80" spans="4:4">
-      <c r="D80" s="13"/>
+      <c r="D80" s="11"/>
     </row>
     <row r="81" spans="4:4">
-      <c r="D81" s="13"/>
+      <c r="D81" s="11"/>
     </row>
     <row r="82" spans="4:4">
-      <c r="D82" s="13"/>
+      <c r="D82" s="11"/>
     </row>
     <row r="83" spans="4:4">
-      <c r="D83" s="13"/>
+      <c r="D83" s="11"/>
     </row>
     <row r="84" spans="4:4">
-      <c r="D84" s="13"/>
+      <c r="D84" s="11"/>
     </row>
     <row r="85" spans="4:4">
-      <c r="D85" s="13"/>
+      <c r="D85" s="11"/>
     </row>
     <row r="86" spans="4:4">
-      <c r="D86" s="13"/>
+      <c r="D86" s="11"/>
     </row>
     <row r="87" spans="4:4">
-      <c r="D87" s="13"/>
+      <c r="D87" s="11"/>
     </row>
     <row r="88" spans="4:4">
-      <c r="D88" s="13"/>
+      <c r="D88" s="11"/>
     </row>
     <row r="89" spans="4:4">
-      <c r="D89" s="13"/>
+      <c r="D89" s="11"/>
     </row>
     <row r="90" spans="4:4">
-      <c r="D90" s="13"/>
+      <c r="D90" s="11"/>
     </row>
     <row r="91" spans="4:4">
-      <c r="D91" s="13"/>
+      <c r="D91" s="11"/>
     </row>
     <row r="92" spans="4:4">
-      <c r="D92" s="13"/>
+      <c r="D92" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1685,7 +1705,7 @@
       </c>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="13">
+      <c r="B3" s="11">
         <v>41348</v>
       </c>
       <c r="C3">
@@ -1693,7 +1713,7 @@
       </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="13">
+      <c r="B4" s="11">
         <v>41409</v>
       </c>
       <c r="C4">
@@ -1701,7 +1721,7 @@
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>41532</v>
       </c>
       <c r="C5">
@@ -1709,7 +1729,7 @@
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>41593</v>
       </c>
       <c r="C6">

</xml_diff>